<commit_message>
Update Andel sysselsatte og registrete ledige ut av bosatte i fylkene SSB 13563 2023.xlsx
oppdateringer
</commit_message>
<xml_diff>
--- a/03_Arbeid og næringsliv/Sysselsetting/2023/Andel sysselsatte og registrete ledige ut av bosatte i fylkene SSB 13563 2023.xlsx
+++ b/03_Arbeid og næringsliv/Sysselsetting/2023/Andel sysselsatte og registrete ledige ut av bosatte i fylkene SSB 13563 2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vestfoldfylke-my.sharepoint.com/personal/ellen_just_hansen_vestfoldfylke_no/Documents/Dokumenter/GitHub/Nyeste Github versjon/Vestfold/03_Arbeid og næringsliv/Sysselsetting/2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="40" documentId="8_{11967D69-27F2-495B-8C18-E23E747167F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3E75E844-47B8-4EED-A954-DFFCF080FEFB}"/>
+  <xr:revisionPtr revIDLastSave="43" documentId="8_{11967D69-27F2-495B-8C18-E23E747167F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{923BC073-09FC-4687-842A-10D7A1BB79D1}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bosatte" sheetId="2" r:id="rId1"/>
@@ -373,7 +373,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="171" formatCode="0.00000"/>
+    <numFmt numFmtId="165" formatCode="0.0\ %"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -436,7 +436,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -743,7 +743,7 @@
   <dimension ref="A1:G106"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+      <selection activeCell="G6" sqref="G6:G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>